<commit_message>
- Got the dataframe _constructor to work - fixed _eval_reindex so that a new dataframe is returned instead of a rating_table instance
</commit_message>
<xml_diff>
--- a/tests/testdata/test_portfolio.xlsx
+++ b/tests/testdata/test_portfolio.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="policy_info" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="driver_info" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="vehicle_info" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="driver_claims" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="rating_inputs_simple" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">driver_claims!$A$1</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="48">
   <si>
     <t xml:space="preserve">policy_number</t>
   </si>
@@ -150,6 +151,27 @@
   </si>
   <si>
     <t xml:space="preserve">02-06-2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Missing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X1</t>
   </si>
 </sst>
 </file>
@@ -166,6 +188,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -261,14 +284,14 @@
   </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -452,11 +475,11 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.98"/>
@@ -496,10 +519,12 @@
       <c r="D2" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="E2" s="3" t="b">
+      <c r="E2" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F2" s="3" t="b">
+      <c r="F2" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G2" s="2"/>
@@ -517,10 +542,12 @@
       <c r="D3" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="E3" s="3" t="b">
+      <c r="E3" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F3" s="3" t="b">
+      <c r="F3" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G3" s="2"/>
@@ -538,10 +565,12 @@
       <c r="D4" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="E4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3" t="b">
+      <c r="E4" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G4" s="2"/>
@@ -559,10 +588,12 @@
       <c r="D5" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="E5" s="3" t="b">
+      <c r="E5" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F5" s="3" t="b">
+      <c r="F5" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G5" s="2"/>
@@ -580,10 +611,12 @@
       <c r="D6" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="E6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3" t="b">
+      <c r="E6" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G6" s="2"/>
@@ -601,10 +634,12 @@
       <c r="D7" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="E7" s="3" t="b">
+      <c r="E7" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F7" s="3" t="b">
+      <c r="F7" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G7" s="2"/>
@@ -612,7 +647,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -627,11 +662,11 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.04"/>
@@ -786,7 +821,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -801,11 +836,11 @@
   </sheetPr>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.72"/>
   </cols>
@@ -1070,7 +1105,97 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>470</v>
+      </c>
+      <c r="B5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>